<commit_message>
Add Ukraine (except Simferopol)
</commit_message>
<xml_diff>
--- a/Owners.xlsx
+++ b/Owners.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255BB553-2162-4F50-84DE-C56545673139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88715C3F-5996-4E9A-BE28-2C8A5C5E1227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{357B1A23-9239-400D-9B56-8A129E784A4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{357B1A23-9239-400D-9B56-8A129E784A4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,9 +288,6 @@
     <t>tt</t>
   </si>
   <si>
-    <t>ukr</t>
-  </si>
-  <si>
     <t>urrv</t>
   </si>
   <si>
@@ -991,6 +988,9 @@
   </si>
   <si>
     <t>miguelalbano</t>
+  </si>
+  <si>
+    <t>uk</t>
   </si>
 </sst>
 </file>
@@ -1350,20 +1350,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC2747D-F3D5-4C0F-8D64-38FAD9ABE72F}">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E8"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="69.6328125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="17.36328125" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="69.5703125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1388,1663 +1387,1674 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>316</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>313</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D62" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D63" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D64" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D65" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D66" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="D67" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D69" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="C71" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="E71" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E71" s="1" t="s">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
-        <v>305</v>
-      </c>
       <c r="B72" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="E72" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E73" s="2"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D74" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E83" s="2"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E84" s="2"/>
     </row>
-    <row r="85" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="C85" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E85" s="2"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E86" s="2"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E87" s="2"/>
-    </row>
-    <row r="88" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
+      <c r="D88" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
+      <c r="D89" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
+      <c r="E90" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E91" s="2"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E92" s="1" t="s">
+      <c r="D94" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E93" s="2"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C96" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E97" s="2"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E98" s="2"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D96" s="2" t="s">
+      <c r="D100" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E96" s="2"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E97" s="2"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E98" s="2"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E99" s="2"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
+      <c r="E100" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
+      <c r="C101" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E101" s="2"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E101" s="2"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="C102" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E102" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D77:E77"/>
     <mergeCell ref="D102:E102"/>
     <mergeCell ref="D61:E61"/>
     <mergeCell ref="D91:E91"/>
@@ -3061,17 +3071,6 @@
     <mergeCell ref="D75:E75"/>
     <mergeCell ref="D76:E76"/>
     <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Khartoum & Juba
</commit_message>
<xml_diff>
--- a/Owners.xlsx
+++ b/Owners.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307F381B-6156-4A8F-8C82-70A56C9B7A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471A939F-3C7A-457A-915E-5220E37F1ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{357B1A23-9239-400D-9B56-8A129E784A4A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="368">
   <si>
     <t>Set</t>
   </si>
@@ -1129,6 +1129,12 @@
   </si>
   <si>
     <t>Area managers without a GitHub account should contact a member of the VATGlasses Team to add updates to the Live &amp; Beta sites. If you'd like to add an area which isn't listed or are responsible for a VATGlasses-managed area, please contact our team for access to the repository.</t>
+  </si>
+  <si>
+    <t>hj-hs</t>
+  </si>
+  <si>
+    <t>Juba, Khartoum</t>
   </si>
 </sst>
 </file>
@@ -1169,10 +1175,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1489,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC2747D-F3D5-4C0F-8D64-38FAD9ABE72F}">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118:E118"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1547,10 +1553,10 @@
       <c r="C3" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1579,10 +1585,10 @@
       <c r="C5" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -1594,10 +1600,10 @@
       <c r="C6" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1864,10 +1870,10 @@
       <c r="C22" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
@@ -2066,10 +2072,10 @@
       <c r="C34" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -2217,253 +2223,251 @@
       <c r="C43" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="E43" s="2"/>
+      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>366</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>125</v>
+        <v>367</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>303</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E44" s="3"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>349</v>
+        <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>350</v>
+        <v>125</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E45" s="2"/>
+        <v>190</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>42</v>
+        <v>349</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>126</v>
+        <v>350</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>303</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>258</v>
+        <v>303</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>199</v>
@@ -2477,161 +2481,161 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>232</v>
+        <v>263</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D66" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>282</v>
-      </c>
+      <c r="E66" s="3"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>62</v>
+        <v>361</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>139</v>
+        <v>362</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>207</v>
+        <v>363</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>277</v>
+        <v>364</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>207</v>
@@ -2645,10 +2649,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>207</v>
@@ -2662,10 +2666,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>207</v>
@@ -2679,10 +2683,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>207</v>
@@ -2696,74 +2700,74 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>342</v>
+        <v>66</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>343</v>
+        <v>143</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>344</v>
+        <v>207</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>345</v>
+        <v>277</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>346</v>
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>67</v>
+        <v>342</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>177</v>
+        <v>343</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E73" s="2"/>
+        <v>344</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E74" s="2"/>
+      <c r="E74" s="3"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>286</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E75" s="3"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>206</v>
@@ -2777,27 +2781,27 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>293</v>
+        <v>70</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>294</v>
+        <v>158</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>289</v>
+        <v>206</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>289</v>
@@ -2811,646 +2815,664 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>71</v>
+        <v>292</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>145</v>
+        <v>288</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E79" s="2"/>
+        <v>289</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>267</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E80" s="3"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E81" s="2"/>
+        <v>208</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D82" s="2" t="s">
+      <c r="C83" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E82" s="2"/>
-    </row>
-    <row r="83" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D83" s="2" t="s">
+      <c r="C84" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E83" s="2"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E84" s="2"/>
+      <c r="E84" s="3"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>75</v>
+        <v>325</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>103</v>
+        <v>326</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>242</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E85" s="3"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>322</v>
+        <v>75</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>323</v>
+        <v>103</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E86" s="2"/>
+        <v>184</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>76</v>
+        <v>322</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>161</v>
+        <v>323</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E87" s="2"/>
+      <c r="D87" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E87" s="3"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>319</v>
+        <v>76</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>318</v>
+        <v>161</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E88" s="2"/>
+      <c r="D88" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E88" s="3"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D89" s="2" t="s">
+      <c r="C90" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E89" s="2"/>
-    </row>
-    <row r="90" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D90" s="2" t="s">
+      <c r="C91" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E90" s="2"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E91" s="2"/>
+      <c r="E91" s="3"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D92" s="2" t="s">
+      <c r="C93" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E92" s="2"/>
-    </row>
-    <row r="93" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E94" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D94" s="2" t="s">
+      <c r="C95" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D95" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E94" s="2"/>
-    </row>
-    <row r="95" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D96" s="2" t="s">
+      <c r="C97" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D97" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E96" s="2"/>
-    </row>
-    <row r="97" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>357</v>
+        <v>80</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>358</v>
+        <v>164</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E99" s="2"/>
+        <v>213</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>330</v>
+        <v>357</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>331</v>
+        <v>358</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>334</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E100" s="3"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>81</v>
+        <v>330</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>165</v>
+        <v>331</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>214</v>
+        <v>332</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>275</v>
+        <v>333</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>276</v>
+        <v>334</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>352</v>
+        <v>81</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>353</v>
+        <v>165</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="E102" s="2"/>
+        <v>214</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>82</v>
+        <v>352</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>166</v>
+        <v>353</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D103" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E103" s="2"/>
+      <c r="D103" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E103" s="3"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>278</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E105" s="2"/>
+        <v>207</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>308</v>
+        <v>84</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>309</v>
+        <v>168</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D106" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E106" s="2"/>
+      <c r="E106" s="3"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>85</v>
+        <v>308</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>169</v>
+        <v>309</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>279</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E107" s="3"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>268</v>
+        <v>85</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>269</v>
+        <v>169</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>270</v>
+        <v>215</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>354</v>
+        <v>268</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>355</v>
+        <v>269</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="E109" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>86</v>
+        <v>354</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>170</v>
+        <v>355</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="E110" s="2"/>
+      <c r="D110" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E110" s="3"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="E111" s="2"/>
+      <c r="D111" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E111" s="3"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E112" s="2"/>
+      <c r="D112" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E112" s="3"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="E113" s="2"/>
+      <c r="D113" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E113" s="3"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>282</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E114" s="3"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E115" s="2"/>
+        <v>216</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E116" s="3"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D116" s="2" t="s">
+      <c r="C117" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D117" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E116" s="2"/>
-    </row>
-    <row r="118" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="3" t="s">
+      <c r="E117" s="3"/>
+    </row>
+    <row r="119" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="A118:E118"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D83:E83"/>
+  <mergeCells count="38">
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D104:E104"/>
     <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
     <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D90:E90"/>
     <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D91:E91"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="A119:E119"/>
     <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D89:E89"/>
     <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D95:E95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Revert "Add Asmara""
This reverts commit e90d8b9387710962db6040295eb543bbec92c37f.
</commit_message>
<xml_diff>
--- a/Owners.xlsx
+++ b/Owners.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696CFE7C-B11A-473B-9333-0D5F9090789B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BC4A1C-B139-45A9-A9B4-A272EE91FFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{357B1A23-9239-400D-9B56-8A129E784A4A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="372">
   <si>
     <t>Set</t>
   </si>
@@ -1141,6 +1141,12 @@
   </si>
   <si>
     <t>Addis Ababa</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>Asmara</t>
   </si>
 </sst>
 </file>
@@ -1501,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC2747D-F3D5-4C0F-8D64-38FAD9ABE72F}">
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:E42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2251,10 +2257,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>178</v>
@@ -2266,246 +2272,244 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>41</v>
+        <v>366</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>125</v>
+        <v>367</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>303</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>349</v>
+        <v>41</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>350</v>
+        <v>125</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E47" s="2"/>
+        <v>190</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>42</v>
+        <v>349</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>126</v>
+        <v>350</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>303</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>258</v>
+        <v>303</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>199</v>
@@ -2519,161 +2523,161 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>232</v>
+        <v>263</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>282</v>
-      </c>
+      <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>62</v>
+        <v>361</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>139</v>
+        <v>362</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>207</v>
+        <v>363</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>277</v>
+        <v>364</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>207</v>
@@ -2687,10 +2691,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>207</v>
@@ -2704,10 +2708,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>207</v>
@@ -2721,10 +2725,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>207</v>
@@ -2738,42 +2742,44 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>342</v>
+        <v>66</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>343</v>
+        <v>143</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>344</v>
+        <v>207</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>345</v>
+        <v>277</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>346</v>
+        <v>278</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>67</v>
+        <v>342</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>177</v>
+        <v>343</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E75" s="2"/>
+        <v>344</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>178</v>
@@ -2785,27 +2791,25 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>286</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>206</v>
@@ -2819,27 +2823,27 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>293</v>
+        <v>70</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>294</v>
+        <v>158</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>289</v>
+        <v>206</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>289</v>
@@ -2853,87 +2857,89 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>71</v>
+        <v>292</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>145</v>
+        <v>288</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E81" s="2"/>
+        <v>289</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>267</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E82" s="2"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E83" s="2"/>
+        <v>208</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D84" s="2" t="s">
+      <c r="C85" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E84" s="2"/>
-    </row>
-    <row r="85" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E85" s="2"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>326</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>178</v>
@@ -2945,72 +2951,72 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>75</v>
+        <v>325</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>103</v>
+        <v>326</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>242</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>322</v>
+        <v>75</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>323</v>
+        <v>103</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E88" s="2"/>
+        <v>184</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>76</v>
+        <v>322</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>161</v>
+        <v>323</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>178</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
       <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>319</v>
+        <v>76</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>318</v>
+        <v>161</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>178</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="E90" s="2"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>160</v>
+        <v>318</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>178</v>
@@ -3020,266 +3026,266 @@
       </c>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D92" s="2" t="s">
+      <c r="C93" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="E92" s="2"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="E93" s="2"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E94" s="2"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D94" s="2" t="s">
+      <c r="C95" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="E94" s="2"/>
-    </row>
-    <row r="95" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D96" s="2" t="s">
+      <c r="C97" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E96" s="2"/>
-    </row>
-    <row r="97" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
+      <c r="E97" s="2"/>
+    </row>
+    <row r="98" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D98" s="2" t="s">
+      <c r="C99" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D99" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E98" s="2"/>
-    </row>
-    <row r="99" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E100" s="1" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>357</v>
+        <v>80</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>358</v>
+        <v>164</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E101" s="2"/>
+        <v>213</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>330</v>
+        <v>357</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>331</v>
+        <v>358</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>334</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E102" s="2"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>81</v>
+        <v>330</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>165</v>
+        <v>331</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>214</v>
+        <v>332</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>275</v>
+        <v>333</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>276</v>
+        <v>334</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>352</v>
+        <v>81</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>353</v>
+        <v>165</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="E104" s="2"/>
+        <v>214</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>82</v>
+        <v>352</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>166</v>
+        <v>353</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>178</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>219</v>
+        <v>356</v>
       </c>
       <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>278</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E106" s="2"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E107" s="2"/>
+        <v>207</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>308</v>
+        <v>84</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>309</v>
+        <v>168</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>178</v>
@@ -3291,210 +3297,226 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>85</v>
+        <v>308</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>169</v>
+        <v>309</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>279</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E109" s="2"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>268</v>
+        <v>85</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>269</v>
+        <v>169</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>270</v>
+        <v>215</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>354</v>
+        <v>268</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>355</v>
+        <v>269</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="E111" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>86</v>
+        <v>354</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>170</v>
+        <v>355</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>178</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>316</v>
+        <v>356</v>
       </c>
       <c r="E112" s="2"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>178</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>287</v>
+        <v>316</v>
       </c>
       <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>178</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>315</v>
+        <v>287</v>
       </c>
       <c r="E114" s="2"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>178</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E115" s="2"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>282</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E116" s="2"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E117" s="2"/>
+        <v>216</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E118" s="2"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D118" s="2" t="s">
+      <c r="C119" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D119" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="E118" s="2"/>
-    </row>
-    <row r="120" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="3" t="s">
+      <c r="E119" s="2"/>
+    </row>
+    <row r="121" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3"/>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A120:E120"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D85:E85"/>
+  <mergeCells count="40">
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D106:E106"/>
     <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
     <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D92:E92"/>
     <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D97:E97"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A121:E121"/>
     <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D91:E91"/>
     <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D84:E84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Combine FSS units into one file
</commit_message>
<xml_diff>
--- a/Owners.xlsx
+++ b/Owners.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BC4A1C-B139-45A9-A9B4-A272EE91FFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F390AA-5894-4491-AE26-AF309D1BC670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{357B1A23-9239-400D-9B56-8A129E784A4A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="366">
   <si>
     <t>Set</t>
   </si>
@@ -48,9 +48,6 @@
     <t>adr</t>
   </si>
   <si>
-    <t>afr</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>bi-bg</t>
   </si>
   <si>
-    <t>car</t>
-  </si>
-  <si>
     <t>dt</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>es</t>
   </si>
   <si>
-    <t>euc</t>
-  </si>
-  <si>
     <t>ev</t>
   </si>
   <si>
@@ -252,9 +243,6 @@
     <t>sa</t>
   </si>
   <si>
-    <t>sam</t>
-  </si>
-  <si>
     <t>sbao</t>
   </si>
   <si>
@@ -312,15 +300,6 @@
     <t>zyz</t>
   </si>
   <si>
-    <t>Caribbean FSS</t>
-  </si>
-  <si>
-    <t>Africa FSS</t>
-  </si>
-  <si>
-    <t>Eurocontrol FSS</t>
-  </si>
-  <si>
     <t>Mauritius</t>
   </si>
   <si>
@@ -339,9 +318,6 @@
     <t>Tahiti</t>
   </si>
   <si>
-    <t>South America FSS</t>
-  </si>
-  <si>
     <t>Falkland Islands/Islas Malvinas</t>
   </si>
   <si>
@@ -708,9 +684,6 @@
     <t>Otto Tuhkunen</t>
   </si>
   <si>
-    <t>Lenny Colton</t>
-  </si>
-  <si>
     <t>Thijs Schepman</t>
   </si>
   <si>
@@ -759,9 +732,6 @@
     <t>seelenkrieger</t>
   </si>
   <si>
-    <t>lennycolton</t>
-  </si>
-  <si>
     <t>gurselalp</t>
   </si>
   <si>
@@ -1147,6 +1117,18 @@
   </si>
   <si>
     <t>Asmara</t>
+  </si>
+  <si>
+    <t>fss</t>
+  </si>
+  <si>
+    <t>Africa, Asia South East, Asia West, Caribbean, Eurocontrol, South America</t>
+  </si>
+  <si>
+    <t>Kieran Hardern</t>
+  </si>
+  <si>
+    <t>KHardern</t>
   </si>
 </sst>
 </file>
@@ -1507,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC2747D-F3D5-4C0F-8D64-38FAD9ABE72F}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45:E45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86:E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1526,7 +1508,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1543,129 +1525,133 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>325</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>147</v>
+        <v>326</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>297</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>93</v>
+        <v>290</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>335</v>
+        <v>295</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>336</v>
+        <v>287</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>297</v>
+        <v>96</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>295</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>296</v>
+        <v>97</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>303</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1673,16 +1659,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1690,33 +1676,33 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1724,33 +1710,33 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>223</v>
+        <v>364</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1758,67 +1744,67 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>226</v>
+        <v>274</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>179</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>284</v>
+        <v>219</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1826,16 +1812,16 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1843,33 +1829,33 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1877,99 +1863,101 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>296</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>115</v>
+        <v>288</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>245</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>306</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>298</v>
+        <v>110</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1977,16 +1965,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1994,16 +1982,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -2011,1512 +1999,1458 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>362</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>119</v>
+        <v>363</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>303</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>337</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>151</v>
+        <v>338</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>303</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>347</v>
+        <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>348</v>
+        <v>113</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>303</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="B41" s="1" t="s">
-        <v>299</v>
+        <v>116</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>360</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>124</v>
+        <v>361</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>303</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>370</v>
+        <v>38</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>371</v>
+        <v>117</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="E45" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>349</v>
+        <v>40</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>350</v>
+        <v>119</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E48" s="2"/>
+        <v>184</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>303</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>259</v>
+        <v>227</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>263</v>
+        <v>223</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>244</v>
+        <v>364</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>243</v>
+        <v>365</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B66" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>242</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E66" s="2"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>60</v>
+        <v>351</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>138</v>
+        <v>352</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>204</v>
+        <v>353</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>240</v>
+        <v>354</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E68" s="2"/>
+        <v>199</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>361</v>
+        <v>60</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>362</v>
+        <v>132</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>363</v>
+        <v>199</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>364</v>
+        <v>267</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>65</v>
+        <v>332</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>142</v>
+        <v>333</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>207</v>
+        <v>334</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>277</v>
+        <v>335</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>278</v>
+        <v>336</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>278</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E74" s="2"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>342</v>
+        <v>65</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>343</v>
+        <v>136</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>346</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>177</v>
+        <v>94</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E76" s="2"/>
+        <v>198</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E77" s="2"/>
+        <v>198</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>69</v>
+        <v>283</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>101</v>
+        <v>284</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>206</v>
+        <v>279</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>70</v>
+        <v>282</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>158</v>
+        <v>278</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>206</v>
+        <v>279</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>293</v>
+        <v>68</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>294</v>
+        <v>137</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>291</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E80" s="2"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>292</v>
+        <v>69</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>288</v>
+        <v>138</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>289</v>
+        <v>200</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E82" s="2"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>72</v>
+        <v>304</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>146</v>
+        <v>303</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>267</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E83" s="2"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>73</v>
+        <v>315</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>102</v>
+        <v>316</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>217</v>
+        <v>305</v>
       </c>
       <c r="E84" s="2"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E85" s="2"/>
-    </row>
-    <row r="86" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>313</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E86" s="2"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>325</v>
+        <v>72</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>326</v>
+        <v>153</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>75</v>
+        <v>309</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>242</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E88" s="2"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>322</v>
+        <v>73</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>323</v>
+        <v>152</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="E89" s="2"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>76</v>
+        <v>201</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>161</v>
+        <v>202</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>302</v>
+        <v>211</v>
       </c>
       <c r="E90" s="2"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>319</v>
+        <v>74</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>318</v>
+        <v>154</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="E91" s="2"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>77</v>
+        <v>310</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>160</v>
+        <v>311</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>209</v>
+        <v>328</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E93" s="2"/>
+        <v>330</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>162</v>
+        <v>203</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>315</v>
+        <v>211</v>
       </c>
       <c r="E94" s="2"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E95" s="2"/>
-    </row>
-    <row r="96" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>338</v>
+        <v>301</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>339</v>
+        <v>302</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>211</v>
+        <v>155</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E97" s="2"/>
-    </row>
-    <row r="98" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+        <v>204</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>310</v>
+        <v>76</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>327</v>
+        <v>156</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>328</v>
+        <v>205</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>329</v>
+        <v>264</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>311</v>
+        <v>347</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>312</v>
+        <v>348</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E99" s="2"/>
     </row>
-    <row r="100" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>304</v>
+        <v>320</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>163</v>
+        <v>321</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>212</v>
+        <v>322</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>265</v>
+        <v>323</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>264</v>
+        <v>324</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>219</v>
+        <v>346</v>
       </c>
       <c r="E102" s="2"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>330</v>
+        <v>78</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>331</v>
+        <v>158</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>334</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E103" s="2"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>352</v>
+        <v>80</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>353</v>
+        <v>160</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>356</v>
+        <v>211</v>
       </c>
       <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>82</v>
+        <v>298</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>166</v>
+        <v>299</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E106" s="2"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>207</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>84</v>
+        <v>258</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>168</v>
+        <v>259</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E108" s="2"/>
+        <v>260</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>308</v>
+        <v>344</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>309</v>
+        <v>345</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>219</v>
+        <v>346</v>
       </c>
       <c r="E109" s="2"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>279</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E110" s="2"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>268</v>
+        <v>83</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>269</v>
+        <v>163</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>272</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E111" s="2"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>354</v>
+        <v>84</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>355</v>
+        <v>164</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>356</v>
+        <v>305</v>
       </c>
       <c r="E112" s="2"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="D113" s="2" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="E114" s="2"/>
+        <v>208</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>315</v>
+        <v>211</v>
       </c>
       <c r="E115" s="2"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="E116" s="2"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A117" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A118" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E118" s="2"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A119" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E119" s="2"/>
-    </row>
-    <row r="121" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3"/>
+    <row r="118" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D68:E68"/>
+  <mergeCells count="37">
+    <mergeCell ref="A118:E118"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D83:E83"/>
     <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
     <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D91:E91"/>
     <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D109:E109"/>
     <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A121:E121"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D84:E84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Move incorrectly placed Owners file
</commit_message>
<xml_diff>
--- a/Owners.xlsx
+++ b/Owners.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="436">
   <si>
     <t>Set</t>
   </si>
@@ -282,337 +282,337 @@
     <t>Lithuania vACC</t>
   </si>
   <si>
+    <t>Patrick Weineis</t>
+  </si>
+  <si>
+    <t>seelenkrieger</t>
+  </si>
+  <si>
+    <t>fa-fd-fx</t>
+  </si>
+  <si>
+    <t>Cape Town, Johannesburg</t>
+  </si>
+  <si>
+    <t>fb</t>
+  </si>
+  <si>
+    <t>Gabrone</t>
+  </si>
+  <si>
+    <t>fc-fe-fg-fk-fo-fp</t>
+  </si>
+  <si>
+    <t>Brazzaville, Douala, Libreville</t>
+  </si>
+  <si>
+    <t>fi-fj</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>fl</t>
+  </si>
+  <si>
+    <t>Lusaka</t>
+  </si>
+  <si>
+    <t>fm</t>
+  </si>
+  <si>
+    <t>Antananarivo</t>
+  </si>
+  <si>
+    <t>fn</t>
+  </si>
+  <si>
+    <t>Luanda</t>
+  </si>
+  <si>
+    <t>fq</t>
+  </si>
+  <si>
+    <t>Beira, Maputo</t>
+  </si>
+  <si>
+    <t>fs</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>fss</t>
+  </si>
+  <si>
+    <t>Africa, Asia South East, Asia West, Caribbean, Eurocontrol, South America</t>
+  </si>
+  <si>
+    <t>Large FSS Position Definitions</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>N'Djamena</t>
+  </si>
+  <si>
+    <t>fv</t>
+  </si>
+  <si>
+    <t>Harare</t>
+  </si>
+  <si>
+    <t>fw</t>
+  </si>
+  <si>
+    <t>Lilongwe</t>
+  </si>
+  <si>
+    <t>fy</t>
+  </si>
+  <si>
+    <t>Windhoek</t>
+  </si>
+  <si>
+    <t>fz</t>
+  </si>
+  <si>
+    <t>Kinshasa, Kisangani, Lubumbashi</t>
+  </si>
+  <si>
+    <t>gc</t>
+  </si>
+  <si>
+    <t>Canarias</t>
+  </si>
+  <si>
+    <t>VATSIM Spain</t>
+  </si>
+  <si>
+    <t>Roger Puig</t>
+  </si>
+  <si>
+    <t>rpuig2001</t>
+  </si>
+  <si>
+    <t>gm</t>
+  </si>
+  <si>
+    <t>Agadir, Casablanca</t>
+  </si>
+  <si>
+    <t>gv</t>
+  </si>
+  <si>
+    <t>Sal</t>
+  </si>
+  <si>
+    <t>ha-hd</t>
+  </si>
+  <si>
+    <t>Addis Ababa</t>
+  </si>
+  <si>
+    <t>vACC Rejected Offer To Participate</t>
+  </si>
+  <si>
+    <t>hb-hr-ht</t>
+  </si>
+  <si>
+    <t>Dar-Es-Salaam</t>
+  </si>
+  <si>
+    <t>hc</t>
+  </si>
+  <si>
+    <t>Mogadishu</t>
+  </si>
+  <si>
+    <t>he</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Egypt vACC</t>
+  </si>
+  <si>
+    <t>Kirollos Nashaat</t>
+  </si>
+  <si>
+    <t>kirollos</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>Asmara</t>
+  </si>
+  <si>
+    <t>hj-hs</t>
+  </si>
+  <si>
+    <t>Juba, Khartoum</t>
+  </si>
+  <si>
+    <t>hk</t>
+  </si>
+  <si>
+    <t>Nairobi</t>
+  </si>
+  <si>
+    <t>hl</t>
+  </si>
+  <si>
+    <t>Tripoli</t>
+  </si>
+  <si>
+    <t>hu</t>
+  </si>
+  <si>
+    <t>Entebbe</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Bulgaria vACC</t>
+  </si>
+  <si>
+    <t>Kristian Karagyozov</t>
+  </si>
+  <si>
+    <t>KristianKaragyozov</t>
+  </si>
+  <si>
+    <t>lc</t>
+  </si>
+  <si>
+    <t>Nicosia</t>
+  </si>
+  <si>
+    <t>Hellenic vACC</t>
+  </si>
+  <si>
+    <t>Spyros Stavrakis</t>
+  </si>
+  <si>
+    <t>SpyrosTTK</t>
+  </si>
+  <si>
+    <t>le</t>
+  </si>
+  <si>
+    <t>Barcelona, Madrid</t>
+  </si>
+  <si>
+    <t>lf</t>
+  </si>
+  <si>
+    <t>Brest, Bordeaux, Marseilles, Paris, Rheims</t>
+  </si>
+  <si>
+    <t>French vACC</t>
+  </si>
+  <si>
+    <t>Corentin Zerbib</t>
+  </si>
+  <si>
+    <t>Pampah91</t>
+  </si>
+  <si>
+    <t>lg</t>
+  </si>
+  <si>
+    <t>Athinai, Makedonia</t>
+  </si>
+  <si>
+    <t>lh</t>
+  </si>
+  <si>
+    <t>Budapest</t>
+  </si>
+  <si>
+    <t>vACCHUN</t>
+  </si>
+  <si>
+    <t>li</t>
+  </si>
+  <si>
+    <t>Brindisi, Milano, Padova, Roma</t>
+  </si>
+  <si>
+    <t>VATSIM Italy</t>
+  </si>
+  <si>
+    <t>Matteo Ferraroni</t>
+  </si>
+  <si>
+    <t>mferraroni</t>
+  </si>
+  <si>
+    <t>lk</t>
+  </si>
+  <si>
+    <t>Praha</t>
+  </si>
+  <si>
+    <t>vACC-CZ</t>
+  </si>
+  <si>
+    <t>lm</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>lo</t>
+  </si>
+  <si>
+    <t>Wien</t>
+  </si>
+  <si>
+    <t>vACC Austria</t>
+  </si>
+  <si>
+    <t>lppc</t>
+  </si>
+  <si>
+    <t>Lisboa</t>
+  </si>
+  <si>
+    <t>Portugal vACC</t>
+  </si>
+  <si>
+    <t>Bernardo Reis</t>
+  </si>
+  <si>
+    <t>becas22</t>
+  </si>
+  <si>
+    <t>lppo</t>
+  </si>
+  <si>
+    <t>Santa Maria</t>
+  </si>
+  <si>
+    <t>lr</t>
+  </si>
+  <si>
+    <t>Bucharest</t>
+  </si>
+  <si>
+    <t>Romania vACC</t>
+  </si>
+  <si>
     <t>Teodor Petrica</t>
   </si>
   <si>
     <t>tgpetrica</t>
-  </si>
-  <si>
-    <t>fa-fd-fx</t>
-  </si>
-  <si>
-    <t>Cape Town, Johannesburg</t>
-  </si>
-  <si>
-    <t>fb</t>
-  </si>
-  <si>
-    <t>Gabrone</t>
-  </si>
-  <si>
-    <t>fc-fe-fg-fk-fo-fp</t>
-  </si>
-  <si>
-    <t>Brazzaville, Douala, Libreville</t>
-  </si>
-  <si>
-    <t>fi-fj</t>
-  </si>
-  <si>
-    <t>Mauritius</t>
-  </si>
-  <si>
-    <t>fl</t>
-  </si>
-  <si>
-    <t>Lusaka</t>
-  </si>
-  <si>
-    <t>fm</t>
-  </si>
-  <si>
-    <t>Antananarivo</t>
-  </si>
-  <si>
-    <t>fn</t>
-  </si>
-  <si>
-    <t>Luanda</t>
-  </si>
-  <si>
-    <t>fq</t>
-  </si>
-  <si>
-    <t>Beira, Maputo</t>
-  </si>
-  <si>
-    <t>fs</t>
-  </si>
-  <si>
-    <t>Seychelles</t>
-  </si>
-  <si>
-    <t>fss</t>
-  </si>
-  <si>
-    <t>Africa, Asia South East, Asia West, Caribbean, Eurocontrol, South America</t>
-  </si>
-  <si>
-    <t>Large FSS Position Definitions</t>
-  </si>
-  <si>
-    <t>ft</t>
-  </si>
-  <si>
-    <t>N'Djamena</t>
-  </si>
-  <si>
-    <t>fv</t>
-  </si>
-  <si>
-    <t>Harare</t>
-  </si>
-  <si>
-    <t>fw</t>
-  </si>
-  <si>
-    <t>Lilongwe</t>
-  </si>
-  <si>
-    <t>fy</t>
-  </si>
-  <si>
-    <t>Windhoek</t>
-  </si>
-  <si>
-    <t>fz</t>
-  </si>
-  <si>
-    <t>Kinshasa, Kisangani, Lubumbashi</t>
-  </si>
-  <si>
-    <t>gc</t>
-  </si>
-  <si>
-    <t>Canarias</t>
-  </si>
-  <si>
-    <t>VATSIM Spain</t>
-  </si>
-  <si>
-    <t>Roger Puig</t>
-  </si>
-  <si>
-    <t>rpuig2001</t>
-  </si>
-  <si>
-    <t>gm</t>
-  </si>
-  <si>
-    <t>Agadir, Casablanca</t>
-  </si>
-  <si>
-    <t>gv</t>
-  </si>
-  <si>
-    <t>Sal</t>
-  </si>
-  <si>
-    <t>ha-hd</t>
-  </si>
-  <si>
-    <t>Addis Ababa</t>
-  </si>
-  <si>
-    <t>vACC Rejected Offer To Participate</t>
-  </si>
-  <si>
-    <t>hb-hr-ht</t>
-  </si>
-  <si>
-    <t>Dar-Es-Salaam</t>
-  </si>
-  <si>
-    <t>hc</t>
-  </si>
-  <si>
-    <t>Mogadishu</t>
-  </si>
-  <si>
-    <t>he</t>
-  </si>
-  <si>
-    <t>Cairo</t>
-  </si>
-  <si>
-    <t>Egypt vACC</t>
-  </si>
-  <si>
-    <t>Kirollos Nashaat</t>
-  </si>
-  <si>
-    <t>kirollos</t>
-  </si>
-  <si>
-    <t>hh</t>
-  </si>
-  <si>
-    <t>Asmara</t>
-  </si>
-  <si>
-    <t>hj-hs</t>
-  </si>
-  <si>
-    <t>Juba, Khartoum</t>
-  </si>
-  <si>
-    <t>hk</t>
-  </si>
-  <si>
-    <t>Nairobi</t>
-  </si>
-  <si>
-    <t>hl</t>
-  </si>
-  <si>
-    <t>Tripoli</t>
-  </si>
-  <si>
-    <t>hu</t>
-  </si>
-  <si>
-    <t>Entebbe</t>
-  </si>
-  <si>
-    <t>lb</t>
-  </si>
-  <si>
-    <t>Sofia</t>
-  </si>
-  <si>
-    <t>Bulgaria vACC</t>
-  </si>
-  <si>
-    <t>Kristian Karagyozov</t>
-  </si>
-  <si>
-    <t>KristianKaragyozov</t>
-  </si>
-  <si>
-    <t>lc</t>
-  </si>
-  <si>
-    <t>Nicosia</t>
-  </si>
-  <si>
-    <t>Hellenic vACC</t>
-  </si>
-  <si>
-    <t>Spyros Stavrakis</t>
-  </si>
-  <si>
-    <t>SpyrosTTK</t>
-  </si>
-  <si>
-    <t>le</t>
-  </si>
-  <si>
-    <t>Barcelona, Madrid</t>
-  </si>
-  <si>
-    <t>lf</t>
-  </si>
-  <si>
-    <t>Brest, Bordeaux, Marseilles, Paris, Rheims</t>
-  </si>
-  <si>
-    <t>French vACC</t>
-  </si>
-  <si>
-    <t>Corentin Zerbib</t>
-  </si>
-  <si>
-    <t>Pampah91</t>
-  </si>
-  <si>
-    <t>lg</t>
-  </si>
-  <si>
-    <t>Athinai, Makedonia</t>
-  </si>
-  <si>
-    <t>lh</t>
-  </si>
-  <si>
-    <t>Budapest</t>
-  </si>
-  <si>
-    <t>vACCHUN</t>
-  </si>
-  <si>
-    <t>Patrick Weineis</t>
-  </si>
-  <si>
-    <t>seelenkrieger</t>
-  </si>
-  <si>
-    <t>li</t>
-  </si>
-  <si>
-    <t>Brindisi, Milano, Padova, Roma</t>
-  </si>
-  <si>
-    <t>VATSIM Italy</t>
-  </si>
-  <si>
-    <t>Matteo Ferraroni</t>
-  </si>
-  <si>
-    <t>mferraroni</t>
-  </si>
-  <si>
-    <t>lk</t>
-  </si>
-  <si>
-    <t>Praha</t>
-  </si>
-  <si>
-    <t>vACC-CZ</t>
-  </si>
-  <si>
-    <t>lm</t>
-  </si>
-  <si>
-    <t>Malta</t>
-  </si>
-  <si>
-    <t>lo</t>
-  </si>
-  <si>
-    <t>Wien</t>
-  </si>
-  <si>
-    <t>vACC Austria</t>
-  </si>
-  <si>
-    <t>lppc</t>
-  </si>
-  <si>
-    <t>Lisboa</t>
-  </si>
-  <si>
-    <t>Portugal vACC</t>
-  </si>
-  <si>
-    <t>Bernardo Reis</t>
-  </si>
-  <si>
-    <t>becas22</t>
-  </si>
-  <si>
-    <t>lppo</t>
-  </si>
-  <si>
-    <t>Santa Maria</t>
-  </si>
-  <si>
-    <t>lr</t>
-  </si>
-  <si>
-    <t>Bucharest</t>
-  </si>
-  <si>
-    <t>Romania vACC</t>
   </si>
   <si>
     <t>ls</t>
@@ -2484,129 +2484,125 @@
         <v>173</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>175</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="D55" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>175</v>
-      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="D58" s="2" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>175</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="D59" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="D61" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -2654,10 +2650,10 @@
         <v>211</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>88</v>
+        <v>197</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>89</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -2688,10 +2684,10 @@
         <v>218</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>175</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">

</xml_diff>